<commit_message>
final commit just aone api left
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\CRM\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C1C99B-51EB-426E-BC10-C105C806AC01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CDB8070-7EA6-4958-862B-BAF77FDBD28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B986BC7B-519A-4E0A-86A3-3CAFF7C30E1C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="226">
   <si>
     <t>http://localhost:3000/client</t>
   </si>
@@ -4868,6 +4868,18 @@
   </si>
   <si>
     <t>edit  paymentMode by id</t>
+  </si>
+  <si>
+    <t>http://localhost:3000/api/admin/quotes-by-employee/{employee ID}</t>
+  </si>
+  <si>
+    <t>get qoutes created by employee</t>
+  </si>
+  <si>
+    <t>get invoices created by employee</t>
+  </si>
+  <si>
+    <t>http://localhost:3000/api/admin/invoices-and-items-by-employee/{employee ID}</t>
   </si>
 </sst>
 </file>
@@ -5305,10 +5317,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9513627A-33A7-4A9F-A044-382CF6846314}">
-  <dimension ref="A1:E227"/>
+  <dimension ref="A1:E229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A213" workbookViewId="0">
-      <selection activeCell="A229" sqref="A229"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B226" sqref="B226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5491,57 +5503,62 @@
         <v>23</v>
       </c>
     </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B13" t="s">
+        <v>223</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>126</v>
+      </c>
+      <c r="E13" s="6"/>
+    </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>78</v>
+        <v>225</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>224</v>
       </c>
       <c r="C14" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D14" t="s">
         <v>126</v>
       </c>
+      <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>126</v>
-      </c>
+      <c r="A15" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>129</v>
+      <c r="A16" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="B16" t="s">
-        <v>130</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D16" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>132</v>
+      <c r="A17" t="s">
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>131</v>
+        <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D17" t="s">
         <v>126</v>
@@ -5549,1280 +5566,1308 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B18" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C18" t="s">
         <v>5</v>
       </c>
       <c r="D18" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B19" t="s">
+        <v>131</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>133</v>
+      </c>
+      <c r="B20" t="s">
+        <v>134</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>136</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B21" t="s">
         <v>137</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C21" t="s">
         <v>138</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D21" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B23" t="s">
         <v>34</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C23" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E23" t="s">
         <v>128</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D22" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
-        <v>70</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D24" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>70</v>
+      </c>
       <c r="D25" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D26" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D27" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D28" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D29" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D30" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D31" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D32" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D33" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D34" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D35" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D36" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D37" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D38" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D39" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D40" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D41" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D42" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="43" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D43" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="44" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D44" s="4" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D45" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="46" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D46" s="4" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="47" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D47" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="48" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D48" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D49" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D50" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D51" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D52" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D53" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D54" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D55" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D56" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D57" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D56" s="3" t="s">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D58" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D57" s="3"/>
-    </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B59" t="s">
-        <v>102</v>
-      </c>
-      <c r="C59" t="s">
-        <v>5</v>
-      </c>
-      <c r="E59" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>103</v>
-      </c>
-      <c r="B60" t="s">
-        <v>104</v>
-      </c>
-      <c r="C60" t="s">
-        <v>5</v>
-      </c>
-      <c r="E60" t="s">
-        <v>128</v>
-      </c>
+      <c r="D59" s="3"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B61" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C61" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E61" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
-        <v>71</v>
+      <c r="A62" t="s">
+        <v>103</v>
       </c>
       <c r="B62" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="C62" t="s">
-        <v>1</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="E62" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D63" s="4" t="s">
-        <v>80</v>
+      <c r="A63" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B63" t="s">
+        <v>106</v>
+      </c>
+      <c r="C63" t="s">
+        <v>3</v>
+      </c>
+      <c r="E63" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D64" s="4" t="s">
-        <v>81</v>
+      <c r="A64" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B64" t="s">
+        <v>79</v>
+      </c>
+      <c r="C64" t="s">
+        <v>1</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E64" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D65" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D66" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D67" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D68" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D69" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D70" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D71" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D72" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D73" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D72" s="3" t="s">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D74" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B76" t="s">
         <v>90</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C76" t="s">
         <v>3</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E76" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A75" s="1" t="s">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B77" t="s">
         <v>92</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C77" t="s">
         <v>11</v>
       </c>
-      <c r="D75" s="3" t="s">
+      <c r="D77" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E75" t="s">
+      <c r="E77" t="s">
         <v>128</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D76" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D77" s="4" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D78" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D79" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D80" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D81" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D82" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D83" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D84" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D85" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D84" s="3" t="s">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D86" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A88" s="1" t="s">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A90" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B90" t="s">
         <v>108</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C90" t="s">
         <v>11</v>
       </c>
-      <c r="D88" s="3" t="s">
+      <c r="D90" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E88" t="s">
+      <c r="E90" t="s">
         <v>128</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D89" s="4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D90" s="4" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D91" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D92" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D93" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D94" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D95" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D96" s="4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D95" s="2"/>
-    </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
+      <c r="D97" s="2"/>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
         <v>114</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B99" t="s">
         <v>115</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C99" t="s">
         <v>1</v>
       </c>
-      <c r="D97" s="7" t="s">
+      <c r="D99" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E97" t="s">
+      <c r="E99" t="s">
         <v>126</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D98" s="8" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D99" s="8" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D100" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D101" s="8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D102" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D103" s="8" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D102" s="7" t="s">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D104" s="7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A104" s="1" t="s">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A106" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B106" t="s">
         <v>221</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C106" t="s">
         <v>11</v>
       </c>
-      <c r="D104" s="7" t="s">
+      <c r="D106" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E104" t="s">
+      <c r="E106" t="s">
         <v>126</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D105" s="8" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D106" s="8" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D107" s="8" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D108" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D109" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D110" s="8" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D109" s="7" t="s">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D111" s="7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A111" t="s">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
         <v>114</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B113" t="s">
         <v>123</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C113" t="s">
         <v>5</v>
-      </c>
-      <c r="E111" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A112" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B112" t="s">
-        <v>124</v>
-      </c>
-      <c r="C112" t="s">
-        <v>5</v>
-      </c>
-      <c r="E112" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A113" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B113" t="s">
-        <v>125</v>
-      </c>
-      <c r="C113" t="s">
-        <v>3</v>
       </c>
       <c r="E113" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A117" s="1" t="s">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A114" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B114" t="s">
+        <v>124</v>
+      </c>
+      <c r="C114" t="s">
+        <v>5</v>
+      </c>
+      <c r="E114" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A115" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B115" t="s">
+        <v>125</v>
+      </c>
+      <c r="C115" t="s">
+        <v>3</v>
+      </c>
+      <c r="E115" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A119" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B119" t="s">
         <v>147</v>
-      </c>
-      <c r="C117" t="s">
-        <v>1</v>
-      </c>
-      <c r="D117" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A118" t="s">
-        <v>140</v>
-      </c>
-      <c r="B118" t="s">
-        <v>141</v>
-      </c>
-      <c r="C118" t="s">
-        <v>1</v>
-      </c>
-      <c r="D118" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A119" t="s">
-        <v>143</v>
-      </c>
-      <c r="B119" t="s">
-        <v>144</v>
       </c>
       <c r="C119" t="s">
         <v>1</v>
       </c>
       <c r="D119" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B120" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C120" t="s">
         <v>1</v>
       </c>
       <c r="D120" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A121" s="1" t="s">
-        <v>154</v>
+      <c r="A121" t="s">
+        <v>143</v>
       </c>
       <c r="B121" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="C121" t="s">
         <v>1</v>
       </c>
       <c r="D121" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B122" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C122" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D122" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A123" t="s">
-        <v>157</v>
+      <c r="A123" s="1" t="s">
+        <v>154</v>
       </c>
       <c r="B123" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C123" t="s">
         <v>1</v>
       </c>
       <c r="D123" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>151</v>
+      </c>
+      <c r="B124" t="s">
+        <v>152</v>
+      </c>
+      <c r="C124" t="s">
+        <v>5</v>
+      </c>
+      <c r="D124" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>157</v>
+      </c>
+      <c r="B125" t="s">
+        <v>158</v>
+      </c>
+      <c r="C125" t="s">
+        <v>1</v>
+      </c>
+      <c r="D125" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A127" t="s">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
         <v>160</v>
       </c>
-      <c r="B127" t="s">
+      <c r="B129" t="s">
         <v>161</v>
       </c>
-      <c r="C127" t="s">
+      <c r="C129" t="s">
         <v>1</v>
       </c>
-      <c r="D127" s="7" t="s">
+      <c r="D129" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E127" t="s">
+      <c r="E129" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D128" s="8" t="s">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D130" s="8" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="129" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D129" s="8" t="s">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D131" s="8" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="130" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D130" s="8" t="s">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D132" s="8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="131" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D131" s="8" t="s">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D133" s="8" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="132" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D132" s="8" t="s">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D134" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="133" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D133" s="8" t="s">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D135" s="8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="134" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D134" s="8" t="s">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D136" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="135" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B135" t="s">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B137" t="s">
         <v>219</v>
       </c>
-      <c r="D135" s="8" t="s">
+      <c r="D137" s="8" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="136" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B136" t="s">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B138" t="s">
         <v>220</v>
       </c>
-      <c r="D136" s="8" t="s">
+      <c r="D138" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="137" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D137" s="8" t="s">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D139" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="138" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D138" s="8" t="s">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D140" s="8" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="139" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D139" s="8" t="s">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D141" s="8" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="140" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D140" s="8" t="s">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D142" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="141" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D141" s="8" t="s">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D143" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="142" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D142" s="8" t="s">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D144" s="8" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="143" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D143" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="144" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D144" s="8" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="145" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D145" s="8" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
     </row>
     <row r="146" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D146" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="147" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D147" s="8" t="s">
-        <v>168</v>
+        <v>63</v>
       </c>
     </row>
     <row r="148" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D148" s="8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="149" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D149" s="8" t="s">
-        <v>57</v>
+        <v>168</v>
       </c>
     </row>
     <row r="150" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D150" s="8" t="s">
-        <v>47</v>
+        <v>169</v>
       </c>
     </row>
     <row r="151" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D151" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="152" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D152" s="8" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="153" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D153" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="154" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D154" s="8" t="s">
-        <v>170</v>
+        <v>59</v>
       </c>
     </row>
     <row r="155" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D155" s="8" t="s">
-        <v>171</v>
+        <v>60</v>
       </c>
     </row>
     <row r="156" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D156" s="8" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="157" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D157" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="158" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D158" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="159" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D159" s="8" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="160" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D160" s="8" t="s">
-        <v>67</v>
+        <v>174</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D161" s="8" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D162" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D163" s="8" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D162" s="7" t="s">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D164" s="7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A165" t="s">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
         <v>177</v>
       </c>
-      <c r="B165" t="s">
+      <c r="B167" t="s">
         <v>178</v>
       </c>
-      <c r="C165" t="s">
+      <c r="C167" t="s">
         <v>5</v>
-      </c>
-      <c r="E165" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A166" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="B166" t="s">
-        <v>180</v>
-      </c>
-      <c r="C166" t="s">
-        <v>5</v>
-      </c>
-      <c r="E166" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A167" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="B167" t="s">
-        <v>182</v>
-      </c>
-      <c r="C167" t="s">
-        <v>1</v>
-      </c>
-      <c r="D167" s="7" t="s">
-        <v>35</v>
       </c>
       <c r="E167" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D168" s="8" t="s">
-        <v>163</v>
+      <c r="A168" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B168" t="s">
+        <v>180</v>
+      </c>
+      <c r="C168" t="s">
+        <v>5</v>
+      </c>
+      <c r="E168" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D169" s="8" t="s">
-        <v>38</v>
+      <c r="A169" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B169" t="s">
+        <v>182</v>
+      </c>
+      <c r="C169" t="s">
+        <v>1</v>
+      </c>
+      <c r="D169" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E169" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D170" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D171" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D172" s="8" t="s">
-        <v>41</v>
+        <v>164</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D173" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D174" s="8" t="s">
-        <v>183</v>
+        <v>41</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D175" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D176" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D177" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D176" s="7" t="s">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D178" s="7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A178" s="1" t="s">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A180" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B178" t="s">
+      <c r="B180" t="s">
         <v>185</v>
       </c>
-      <c r="C178" t="s">
+      <c r="C180" t="s">
         <v>3</v>
       </c>
-      <c r="E178" t="s">
+      <c r="E180" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A179" s="1" t="s">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A181" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B179" t="s">
+      <c r="B181" t="s">
         <v>187</v>
       </c>
-      <c r="C179" t="s">
+      <c r="C181" t="s">
         <v>1</v>
       </c>
-      <c r="D179" s="7" t="s">
+      <c r="D181" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E179" t="s">
+      <c r="E181" t="s">
         <v>176</v>
-      </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D180" s="8" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D181" s="8" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D182" s="8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D183" s="8" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D184" s="8" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D185" s="8" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D186" s="8" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D187" s="8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D188" s="8" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D189" s="8" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D190" s="8" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D189" s="7" t="s">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D191" s="7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A191" s="1" t="s">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A193" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="B191" t="s">
+      <c r="B193" t="s">
         <v>198</v>
       </c>
-      <c r="C191" t="s">
+      <c r="C193" t="s">
         <v>3</v>
       </c>
-      <c r="D191" s="7" t="s">
+      <c r="D193" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E191" t="s">
+      <c r="E193" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A192" s="1" t="s">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A194" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B192" t="s">
+      <c r="B194" t="s">
         <v>200</v>
       </c>
-      <c r="C192" t="s">
+      <c r="C194" t="s">
         <v>11</v>
       </c>
-      <c r="D192" s="8" t="s">
+      <c r="D194" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="E192" t="s">
+      <c r="E194" t="s">
         <v>176</v>
-      </c>
-    </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D193" s="8" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D194" s="8" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D195" s="8" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D196" s="8" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D197" s="8" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D198" s="8" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D199" s="8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D200" s="8" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D201" s="8" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D202" s="8" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D201" s="7" t="s">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D203" s="7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A206" t="s">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A208" t="s">
         <v>201</v>
       </c>
-      <c r="B206" t="s">
+      <c r="B208" t="s">
         <v>208</v>
       </c>
-      <c r="C206" t="s">
+      <c r="C208" t="s">
         <v>1</v>
       </c>
-      <c r="D206" s="7" t="s">
+      <c r="D208" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E206" t="s">
+      <c r="E208" t="s">
         <v>176</v>
-      </c>
-    </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D207" s="8" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D208" s="8" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D209" s="8" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D210" s="8" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D211" s="8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D212" s="8" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D213" s="8" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D214" s="8" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D213" s="7" t="s">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D215" s="7" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A216" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="B216" t="s">
-        <v>209</v>
-      </c>
-      <c r="C216" t="s">
-        <v>5</v>
-      </c>
-      <c r="D216" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A217" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="B217" t="s">
-        <v>212</v>
-      </c>
-      <c r="C217" t="s">
-        <v>5</v>
-      </c>
-      <c r="D217" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B218" t="s">
+        <v>209</v>
+      </c>
+      <c r="C218" t="s">
+        <v>5</v>
+      </c>
+      <c r="D218" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A219" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B219" t="s">
+        <v>212</v>
+      </c>
+      <c r="C219" t="s">
+        <v>5</v>
+      </c>
+      <c r="D219" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A220" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="B218" t="s">
+      <c r="B220" t="s">
         <v>214</v>
       </c>
-      <c r="C218" t="s">
+      <c r="C220" t="s">
         <v>215</v>
       </c>
-      <c r="D218" s="7" t="s">
+      <c r="D220" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E218" t="s">
+      <c r="E220" t="s">
         <v>176</v>
-      </c>
-    </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D219" s="8" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D220" s="8" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D221" s="8" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D222" s="8" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D223" s="8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D224" s="8" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D225" s="8" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D226" s="8" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D225" s="7" t="s">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D227" s="7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A227" s="1" t="s">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A229" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B227" t="s">
+      <c r="B229" t="s">
         <v>217</v>
       </c>
-      <c r="C227" t="s">
+      <c r="C229" t="s">
         <v>3</v>
       </c>
-      <c r="D227" t="s">
+      <c r="D229" t="s">
         <v>176</v>
       </c>
     </row>
@@ -6832,34 +6877,36 @@
     <hyperlink ref="A4" r:id="rId2" xr:uid="{C78BF9C7-BE75-43E6-ABFE-B17E62613710}"/>
     <hyperlink ref="A5" r:id="rId3" xr:uid="{79FC1B8B-B838-4852-8C29-1F3200A11AD4}"/>
     <hyperlink ref="A10" r:id="rId4" xr:uid="{55D52392-34F7-463F-B4F2-85613443566F}"/>
-    <hyperlink ref="A14" r:id="rId5" xr:uid="{DA1E5DC3-A62D-463F-8A5D-09AA6AF1FDC1}"/>
-    <hyperlink ref="A62" r:id="rId6" xr:uid="{15EE56A5-E50E-4D8B-9383-F7B405A03AD4}"/>
+    <hyperlink ref="A16" r:id="rId5" xr:uid="{DA1E5DC3-A62D-463F-8A5D-09AA6AF1FDC1}"/>
+    <hyperlink ref="A64" r:id="rId6" xr:uid="{15EE56A5-E50E-4D8B-9383-F7B405A03AD4}"/>
     <hyperlink ref="A6" r:id="rId7" xr:uid="{4FCF2571-39DA-4841-912E-02FA8F24B683}"/>
     <hyperlink ref="A12" r:id="rId8" xr:uid="{1296D6E9-F63F-47F7-8035-8F2F378A176D}"/>
-    <hyperlink ref="A21" r:id="rId9" xr:uid="{35B6F2DF-8DE3-4451-AF56-69C56A776292}"/>
-    <hyperlink ref="A74" r:id="rId10" xr:uid="{4B921DD1-899D-4D56-B765-265E6BB39B64}"/>
-    <hyperlink ref="A75" r:id="rId11" xr:uid="{88EDFC72-2E33-4D0E-88BD-69CDB982D3B4}"/>
-    <hyperlink ref="A59" r:id="rId12" xr:uid="{1977F374-0548-4A59-B7C7-D6F2842B777B}"/>
-    <hyperlink ref="A61" r:id="rId13" xr:uid="{314BB1CF-CD8B-4256-9D91-7EEC20D9C15D}"/>
-    <hyperlink ref="A88" r:id="rId14" xr:uid="{DDDF7408-861E-4BCB-88C3-A8871B1BE886}"/>
-    <hyperlink ref="A104" r:id="rId15" xr:uid="{E7138814-4FAB-443B-8320-C80BCDB57CA5}"/>
-    <hyperlink ref="A112" r:id="rId16" xr:uid="{15966464-DDCC-4B0E-8B65-1AC38725E53C}"/>
-    <hyperlink ref="A113" r:id="rId17" xr:uid="{2ED4D440-73AA-4D91-A2DC-FDB85F1A3EA1}"/>
-    <hyperlink ref="A17" r:id="rId18" xr:uid="{75DD6973-632E-4534-8563-E18568C9A146}"/>
-    <hyperlink ref="A117" r:id="rId19" xr:uid="{8EDAB16F-7623-495C-9D13-F810C866876D}"/>
-    <hyperlink ref="A121" r:id="rId20" xr:uid="{F004F29D-1D32-436D-8755-05FE0B9232DB}"/>
-    <hyperlink ref="A166" r:id="rId21" xr:uid="{D9F27E28-2A74-4207-AD56-42457B896BF6}"/>
-    <hyperlink ref="A167" r:id="rId22" xr:uid="{6AAF855E-CE18-4396-BE63-5BB3332F98D8}"/>
-    <hyperlink ref="A178" r:id="rId23" xr:uid="{49A73C62-A272-4241-AA24-BF2B1296F857}"/>
-    <hyperlink ref="A179" r:id="rId24" xr:uid="{DB4C2684-621A-4564-9409-00BAC47DF969}"/>
-    <hyperlink ref="A191" r:id="rId25" xr:uid="{9C05DD0F-8309-41E0-B609-CA13C0494681}"/>
-    <hyperlink ref="A192" r:id="rId26" xr:uid="{E9FEA33C-36BA-49DD-A3AF-9139C3C35B79}"/>
-    <hyperlink ref="A216" r:id="rId27" xr:uid="{156BAC8A-0F79-4C5E-B26E-5A592EC96D69}"/>
-    <hyperlink ref="A217" r:id="rId28" xr:uid="{CCB28DFF-280E-4119-9CD7-E8095AC8EB69}"/>
-    <hyperlink ref="A218" r:id="rId29" xr:uid="{4F99BD7E-7800-4653-9895-58E3AAE83A0E}"/>
-    <hyperlink ref="A227" r:id="rId30" xr:uid="{84FF0F89-A3EA-4402-A8E9-469DB20B52F3}"/>
+    <hyperlink ref="A23" r:id="rId9" xr:uid="{35B6F2DF-8DE3-4451-AF56-69C56A776292}"/>
+    <hyperlink ref="A76" r:id="rId10" xr:uid="{4B921DD1-899D-4D56-B765-265E6BB39B64}"/>
+    <hyperlink ref="A77" r:id="rId11" xr:uid="{88EDFC72-2E33-4D0E-88BD-69CDB982D3B4}"/>
+    <hyperlink ref="A61" r:id="rId12" xr:uid="{1977F374-0548-4A59-B7C7-D6F2842B777B}"/>
+    <hyperlink ref="A63" r:id="rId13" xr:uid="{314BB1CF-CD8B-4256-9D91-7EEC20D9C15D}"/>
+    <hyperlink ref="A90" r:id="rId14" xr:uid="{DDDF7408-861E-4BCB-88C3-A8871B1BE886}"/>
+    <hyperlink ref="A106" r:id="rId15" xr:uid="{E7138814-4FAB-443B-8320-C80BCDB57CA5}"/>
+    <hyperlink ref="A114" r:id="rId16" xr:uid="{15966464-DDCC-4B0E-8B65-1AC38725E53C}"/>
+    <hyperlink ref="A115" r:id="rId17" xr:uid="{2ED4D440-73AA-4D91-A2DC-FDB85F1A3EA1}"/>
+    <hyperlink ref="A19" r:id="rId18" xr:uid="{75DD6973-632E-4534-8563-E18568C9A146}"/>
+    <hyperlink ref="A119" r:id="rId19" xr:uid="{8EDAB16F-7623-495C-9D13-F810C866876D}"/>
+    <hyperlink ref="A123" r:id="rId20" xr:uid="{F004F29D-1D32-436D-8755-05FE0B9232DB}"/>
+    <hyperlink ref="A168" r:id="rId21" xr:uid="{D9F27E28-2A74-4207-AD56-42457B896BF6}"/>
+    <hyperlink ref="A169" r:id="rId22" xr:uid="{6AAF855E-CE18-4396-BE63-5BB3332F98D8}"/>
+    <hyperlink ref="A180" r:id="rId23" xr:uid="{49A73C62-A272-4241-AA24-BF2B1296F857}"/>
+    <hyperlink ref="A181" r:id="rId24" xr:uid="{DB4C2684-621A-4564-9409-00BAC47DF969}"/>
+    <hyperlink ref="A193" r:id="rId25" xr:uid="{9C05DD0F-8309-41E0-B609-CA13C0494681}"/>
+    <hyperlink ref="A194" r:id="rId26" xr:uid="{E9FEA33C-36BA-49DD-A3AF-9139C3C35B79}"/>
+    <hyperlink ref="A218" r:id="rId27" xr:uid="{156BAC8A-0F79-4C5E-B26E-5A592EC96D69}"/>
+    <hyperlink ref="A219" r:id="rId28" xr:uid="{CCB28DFF-280E-4119-9CD7-E8095AC8EB69}"/>
+    <hyperlink ref="A220" r:id="rId29" xr:uid="{4F99BD7E-7800-4653-9895-58E3AAE83A0E}"/>
+    <hyperlink ref="A229" r:id="rId30" xr:uid="{84FF0F89-A3EA-4402-A8E9-469DB20B52F3}"/>
+    <hyperlink ref="A13" r:id="rId31" xr:uid="{E43716C5-88D8-4F9C-8D3A-5DC2CD45F5AE}"/>
+    <hyperlink ref="A14" r:id="rId32" xr:uid="{7273D24B-ECE5-42CE-A231-0A552E321BFE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId31"/>
+  <pageSetup orientation="portrait" r:id="rId33"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
pdf data fetch api
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\CRM\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A67444C-88E9-404F-B0FA-8DC328B25B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F4AE13-94B6-41BC-BCA0-57656DAA79A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B986BC7B-519A-4E0A-86A3-3CAFF7C30E1C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="369">
   <si>
     <t>http://localhost:3000/client</t>
   </si>
@@ -7245,6 +7245,3486 @@
   </si>
   <si>
     <t>http://localhost:3000/api/reports/accounts</t>
+  </si>
+  <si>
+    <t>get all the things of qoute for pdf creation by id</t>
+  </si>
+  <si>
+    <r>
+      <t>    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"message"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Quote PDF details generated successfully"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"data"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"quoteData"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"id"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"client_id"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"number"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"1691497399368-7635"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"quote_current_date"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"2023-08-07T19:00:00.000Z"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"added_by_employee"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"expiry_date"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"2023-12-30T19:00:00.000Z"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"execution_time"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"2 weeks"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"bank_details"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Bank details..."</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"payment_mode_id"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"pdf_file_name"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"quote_1.pdf"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"client_email"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"john.doe@example.com"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"employee_email"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"123456789@example.com"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"quoteItems"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>[</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"id"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"quote_id"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"item_name"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Item 1"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"item_description"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Description for Item 1"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"item_quantity"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"item_xdim"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"item_ydim"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>15</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"item_price"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"item_subtotal"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>200</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"item_tax"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"item_total"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>220</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>},</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"id"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"item_name"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Item 2"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"item_description"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Description for Item 2"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"item_quantity"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"item_xdim"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"item_ydim"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"item_price"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"item_subtotal"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>150</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"item_tax"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>15</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>                </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"item_total"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>165</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>],</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"settings"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"logo_img"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>null</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"stamp_img"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"img.png"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"name"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"New VAT number here"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"address"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"New VAT number here"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"vat_no"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"New VAT number here"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"id"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"client"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"fname"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"John"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"lname"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"John"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"phone"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"1234567890"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"email"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"john.doe@example.com"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"date"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>null</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"added_by_employee"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>null</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"company_name"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>null</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"employee"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"name"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"John"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"surname"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Doe"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"birthday"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"1989-12-31T19:00:00.000Z"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"department"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"accounts"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"position"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Manager"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"email"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"123456789@example.com"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"password"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"$2b$10$b3XluLRrDUX.vOI7krgfauiOYjUhCEzjmQJE/mNeXzocLaUzYfxjS"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"status"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Draft"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"paymentMode"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"name"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Credit Card"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"description"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Payment via credit card"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"is_enabled"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"is_default"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Summarry"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"subtotal"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>385</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"vatRate"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"tax"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>38.5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"total"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDCDCDC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>423.5</t>
+    </r>
+  </si>
+  <si>
+    <t>authToken admin/sales</t>
+  </si>
+  <si>
+    <t>get invoice pdf data by id</t>
+  </si>
+  <si>
+    <t>http://localhost:3000/api/invoice/{invoice id}/pdf</t>
+  </si>
+  <si>
+    <t>http://localhost:3000/api/quote/{quote id}/pdf</t>
+  </si>
+  <si>
+    <t>authToken admin/accounts</t>
   </si>
 </sst>
 </file>
@@ -7682,10 +11162,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9513627A-33A7-4A9F-A044-382CF6846314}">
-  <dimension ref="A1:E334"/>
+  <dimension ref="A1:E432"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="C422" workbookViewId="0">
+      <selection activeCell="E431" sqref="E431"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9721,74 +13201,569 @@
         <v>282</v>
       </c>
     </row>
-    <row r="321" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E321" s="8" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="322" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E322" s="8" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="323" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E323" s="8" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="324" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E324" s="8" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="325" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E325" s="8" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="326" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E326" s="8" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="327" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E327" s="8" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="328" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E328" s="8" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="329" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E329" s="8" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="330" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E330" s="8" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="331" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E331" s="8" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="332" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E332" s="8" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="333" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E333" s="8" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="334" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E334" s="7" t="s">
         <v>69</v>
+      </c>
+    </row>
+    <row r="336" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A336" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="B336" t="s">
+        <v>288</v>
+      </c>
+      <c r="C336" t="s">
+        <v>5</v>
+      </c>
+      <c r="D336" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E336" s="8" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="337" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D337" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="338" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D338" s="8" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="339" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D339" s="8" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="340" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D340" s="8" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="341" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D341" s="8" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="342" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D342" s="8" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="343" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D343" s="8" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="344" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D344" s="8" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="345" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D345" s="8" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="346" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D346" s="8" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="347" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D347" s="8" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="348" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D348" s="8" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="349" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D349" s="8" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="350" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D350" s="8" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="351" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D351" s="8" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="352" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D352" s="8" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="353" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D353" s="8" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="354" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D354" s="8" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="355" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D355" s="8" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="356" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D356" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="357" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D357" s="8" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="358" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D358" s="8" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="359" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D359" s="8" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="360" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D360" s="8" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="361" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D361" s="8" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="362" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D362" s="8" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="363" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D363" s="8" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="364" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D364" s="8" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="365" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D365" s="8" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="366" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D366" s="8" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="367" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D367" s="8" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="368" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D368" s="8" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="369" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D369" s="8" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="370" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D370" s="8" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="371" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D371" s="8" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="372" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D372" s="8" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="373" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D373" s="8" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="374" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D374" s="8" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="375" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D375" s="8" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="376" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D376" s="8" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="377" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D377" s="8" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="378" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D378" s="8" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="379" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D379" s="8" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="380" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D380" s="8" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="381" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D381" s="8" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="382" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D382" s="8" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="383" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D383" s="8" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="384" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D384" s="8" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="385" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D385" s="8" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="386" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D386" s="8" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="387" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D387" s="8" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="388" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D388" s="8" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="389" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D389" s="8" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="390" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D390" s="8" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="391" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D391" s="8" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="392" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D392" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="393" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D393" s="8" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="394" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D394" s="8" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="395" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D395" s="8" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="396" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D396" s="8" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="397" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D397" s="8" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="398" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D398" s="8" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="399" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D399" s="8" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="400" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D400" s="8" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="401" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D401" s="8" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="402" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D402" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="403" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D403" s="8" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="404" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D404" s="8" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="405" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D405" s="8" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="406" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D406" s="8" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="407" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D407" s="8" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="408" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D408" s="8" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="409" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D409" s="8" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="410" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D410" s="8" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="411" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D411" s="8" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="412" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D412" s="8" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="413" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D413" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="414" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D414" s="8" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="415" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D415" s="8" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="416" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D416" s="8" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="417" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D417" s="8" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="418" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D418" s="8" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="419" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D419" s="8" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="420" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D420" s="8" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="421" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D421" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="422" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D422" s="8" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="423" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D423" s="8" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="424" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D424" s="8" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="425" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D425" s="8" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="426" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D426" s="8" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="427" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D427" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="428" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D428" s="8" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="429" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D429" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="431" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E431" s="8" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="432" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A432" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="B432" t="s">
+        <v>365</v>
       </c>
     </row>
   </sheetData>
@@ -9828,8 +13803,10 @@
     <hyperlink ref="A316" r:id="rId33" xr:uid="{46D0FF6B-B024-48CB-9956-1B66B450639D}"/>
     <hyperlink ref="A7" r:id="rId34" xr:uid="{6ABFC4A8-EE37-487F-BC65-4776B37F54D9}"/>
     <hyperlink ref="A9" r:id="rId35" xr:uid="{3C77D7FF-CD0D-4ECA-86DC-039EA8E8FA34}"/>
+    <hyperlink ref="A432" r:id="rId36" xr:uid="{BE6FC797-4111-47EF-8F19-86BCF58E5060}"/>
+    <hyperlink ref="A336" r:id="rId37" xr:uid="{8D2B771A-3EE4-4CE5-BAC4-8E1341E093F5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId36"/>
+  <pageSetup orientation="portrait" r:id="rId38"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updaed backend small  bug fix
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\CRM_FrontEnd\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09917EDD-728B-4A6F-B0DF-F743C0EF2CF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB0FFB3-02CC-4BC1-A5D0-B9CDD791362E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B986BC7B-519A-4E0A-86A3-3CAFF7C30E1C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="395">
   <si>
     <t>http://localhost:3000/client</t>
   </si>
@@ -10911,13 +10911,19 @@
   </si>
   <si>
     <t>form data (pdfFile,employeeId,clientId,employeePassword)</t>
+  </si>
+  <si>
+    <t>2 = &gt; accepted, 3= &gt; rejected</t>
+  </si>
+  <si>
+    <t>0 NO ,1 pending ,2 accepted,3 rejected</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -10975,6 +10981,12 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF6A9955"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -11009,7 +11021,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -11034,6 +11046,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -11353,8 +11368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9513627A-33A7-4A9F-A044-382CF6846314}">
   <dimension ref="A1:E446"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B232" workbookViewId="0">
-      <selection activeCell="B444" sqref="B444"/>
+    <sheetView tabSelected="1" topLeftCell="A426" workbookViewId="0">
+      <selection activeCell="A435" sqref="A435"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13999,11 +14014,17 @@
       </c>
     </row>
     <row r="437" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B437" t="s">
+        <v>393</v>
+      </c>
       <c r="D437" s="8" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="438" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B438" s="10" t="s">
+        <v>394</v>
+      </c>
       <c r="D438" s="7" t="s">
         <v>68</v>
       </c>

</xml_diff>

<commit_message>
client add(error employee name) added
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\CRM_FrontEnd\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A45F6C-6B74-4338-91EC-F63AF06FD711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92AD62D6-F17D-4363-B4FC-D108FAF5375E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B986BC7B-519A-4E0A-86A3-3CAFF7C30E1C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="406">
   <si>
     <t>http://localhost:3000/client</t>
   </si>
@@ -11164,6 +11164,18 @@
       </rPr>
       <t>"admin123"</t>
     </r>
+  </si>
+  <si>
+    <t>http://localhost:3000/api/employee/clients</t>
+  </si>
+  <si>
+    <t>get clients added by specific emp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">get </t>
+  </si>
+  <si>
+    <t>emp token</t>
   </si>
 </sst>
 </file>
@@ -11613,10 +11625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9513627A-33A7-4A9F-A044-382CF6846314}">
-  <dimension ref="A1:E453"/>
+  <dimension ref="A1:E455"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A435" workbookViewId="0">
-      <selection activeCell="B457" sqref="B457"/>
+      <selection activeCell="D455" sqref="D455"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14375,29 +14387,43 @@
         <v>397</v>
       </c>
     </row>
-    <row r="449" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D449" s="8" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="450" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="450" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D450" s="8" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="451" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="451" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D451" s="8" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="452" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="452" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D452" s="8" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="453" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="453" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D453" s="7" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="455" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A455" t="s">
+        <v>402</v>
+      </c>
+      <c r="B455" t="s">
+        <v>403</v>
+      </c>
+      <c r="C455" t="s">
+        <v>404</v>
+      </c>
+      <c r="D455" s="8" t="s">
+        <v>405</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sales/account employee get api
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\CRM_FrontEnd\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23A57AB-745E-48C2-869B-6A0348B673EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98648F16-5EA8-48EC-9BB8-60046F77D93B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B986BC7B-519A-4E0A-86A3-3CAFF7C30E1C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="426">
   <si>
     <t>http://localhost:3000/client</t>
   </si>
@@ -11669,9 +11669,6 @@
     <t>http://localhost:3000/api/quote/convertQuoteToInvoice</t>
   </si>
   <si>
-    <t>convert quote to invoice and assign it to specifiv employee</t>
-  </si>
-  <si>
     <r>
       <t> </t>
     </r>
@@ -11743,6 +11740,21 @@
       </rPr>
       <t>"sharjeel@gmail.com"</t>
     </r>
+  </si>
+  <si>
+    <t>convert quote to invoice and assign it to specific employee</t>
+  </si>
+  <si>
+    <t>http://localhost:3000/api/admin/all-salesEmployees</t>
+  </si>
+  <si>
+    <t>get all sales employee</t>
+  </si>
+  <si>
+    <t>get all accounts employee</t>
+  </si>
+  <si>
+    <t>http://localhost:3000/api/admin/all-accountsEmployees</t>
   </si>
 </sst>
 </file>
@@ -12192,10 +12204,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9513627A-33A7-4A9F-A044-382CF6846314}">
-  <dimension ref="A2:E474"/>
+  <dimension ref="A2:E477"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A455" workbookViewId="0">
-      <selection activeCell="B460" sqref="B460"/>
+    <sheetView tabSelected="1" topLeftCell="A456" workbookViewId="0">
+      <selection activeCell="A479" sqref="A479"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15072,7 +15084,7 @@
         <v>418</v>
       </c>
       <c r="B471" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="C471" t="s">
         <v>13</v>
@@ -15083,17 +15095,39 @@
     </row>
     <row r="472" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D472" s="8" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="473" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D473" s="8" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="474" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D474" s="7" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="476" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A476" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="B476" t="s">
+        <v>423</v>
+      </c>
+      <c r="C476" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="477" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A477" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="B477" t="s">
+        <v>424</v>
+      </c>
+      <c r="C477" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -15143,8 +15177,10 @@
     <hyperlink ref="A456" r:id="rId43" xr:uid="{2B6879B5-B082-439F-9722-96D81989E606}"/>
     <hyperlink ref="A457" r:id="rId44" xr:uid="{C600E6E0-892F-46FF-AF20-F0B68C77007A}"/>
     <hyperlink ref="A467" r:id="rId45" xr:uid="{D1B98F0C-1BFD-402A-A280-18488EE1147C}"/>
+    <hyperlink ref="A476" r:id="rId46" xr:uid="{633D7BF7-A5D7-4BA1-9EFA-C7411599728C}"/>
+    <hyperlink ref="A477" r:id="rId47" xr:uid="{621BF094-0F40-4B27-B035-C3C25A20EE38}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId46"/>
+  <pageSetup orientation="portrait" r:id="rId48"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
just lpo left discount added
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\CRM_FrontEnd\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98648F16-5EA8-48EC-9BB8-60046F77D93B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A681B307-E109-4E63-99C9-21594DD0262B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B986BC7B-519A-4E0A-86A3-3CAFF7C30E1C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="428">
   <si>
     <t>http://localhost:3000/client</t>
   </si>
@@ -11755,6 +11755,12 @@
   </si>
   <si>
     <t>http://localhost:3000/api/admin/all-accountsEmployees</t>
+  </si>
+  <si>
+    <t>http://localhost:3000/api/quote/getAllApprovedByClientQuotes</t>
+  </si>
+  <si>
+    <t>get quote which are approved by client and not assigned to any employee</t>
   </si>
 </sst>
 </file>
@@ -12204,16 +12210,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9513627A-33A7-4A9F-A044-382CF6846314}">
-  <dimension ref="A2:E477"/>
+  <dimension ref="A2:E478"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A456" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A347" workbookViewId="0">
       <selection activeCell="A479" sqref="A479"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="68.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="76.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="49.21875" bestFit="1" customWidth="1"/>
@@ -15127,6 +15133,17 @@
         <v>424</v>
       </c>
       <c r="C477" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="478" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A478" t="s">
+        <v>426</v>
+      </c>
+      <c r="B478" t="s">
+        <v>427</v>
+      </c>
+      <c r="C478" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>